<commit_message>
Diagram can be drawn in SVG, and it is helpful to look at.
</commit_message>
<xml_diff>
--- a/Bernina day timetable.xlsx
+++ b/Bernina day timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ba76bc22b2fda58/Documents/Holiday 2024 Interrail/ZigZagTimetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE6934CB-C600-4209-BB10-9DA06E7E5674}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69615A79-858B-44D6-879A-FADDB6A48403}"/>
   <bookViews>
-    <workbookView xWindow="1886" yWindow="1886" windowWidth="8434" windowHeight="9763" firstSheet="1" activeTab="1" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
+    <workbookView xWindow="1886" yWindow="1886" windowWidth="11820" windowHeight="10234" firstSheet="1" activeTab="1" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Direct trains" sheetId="1" r:id="rId1"/>
@@ -1381,7 +1381,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1447,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -1455,7 +1455,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Added more train times. Removed placeholder lines from initial SVG.
</commit_message>
<xml_diff>
--- a/Bernina day timetable.xlsx
+++ b/Bernina day timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ba76bc22b2fda58/Documents/Holiday 2024 Interrail/ZigZagTimetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69615A79-858B-44D6-879A-FADDB6A48403}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64E9557A-8B2B-43E2-AE1A-6EF87906A031}"/>
   <bookViews>
-    <workbookView xWindow="1886" yWindow="1886" windowWidth="11820" windowHeight="10234" firstSheet="1" activeTab="1" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
+    <workbookView xWindow="3386" yWindow="5357" windowWidth="18823" windowHeight="10234" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Direct trains" sheetId="1" r:id="rId1"/>
@@ -37,15 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="17">
   <si>
     <t>From</t>
-  </si>
-  <si>
-    <t>Depart</t>
-  </si>
-  <si>
-    <t>Arrive</t>
   </si>
   <si>
     <t>Bologna</t>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Depart decimal minnutes</t>
+  </si>
+  <si>
+    <t>Arrive decimal</t>
   </si>
 </sst>
 </file>
@@ -478,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C10AF06-4BAA-4E39-BA8A-BDC99B314CB9}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -496,27 +496,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>456</v>
@@ -529,16 +529,16 @@
         <v>4.9333333333333336</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" ref="F2:F31" si="0">ROUNDDOWN(D2/100,0) +MOD(D2,100)/60</f>
+        <f t="shared" ref="F2:F38" si="0">ROUNDDOWN(D2/100,0) +MOD(D2,100)/60</f>
         <v>7.083333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>506</v>
@@ -547,7 +547,7 @@
         <v>712</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E15" si="1">ROUNDDOWN(C3/100,0) +MOD(C3,100)/60</f>
+        <f t="shared" ref="E3:E19" si="1">ROUNDDOWN(C3/100,0) +MOD(C3,100)/60</f>
         <v>5.0999999999999996</v>
       </c>
       <c r="F3" s="2">
@@ -557,10 +557,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>731</v>
@@ -579,10 +579,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>731</v>
@@ -601,774 +601,994 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>720</v>
+        <v>836</v>
       </c>
       <c r="D6" s="1">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>7.333333333333333</v>
+        <v>8.6</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>9.8666666666666671</v>
+        <v>9.8333333333333339</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>820</v>
+        <v>856</v>
       </c>
       <c r="D7" s="1">
-        <v>1052</v>
+        <v>1000</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="1"/>
-        <v>8.3333333333333339</v>
+        <v>8.9333333333333336</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>10.866666666666667</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>920</v>
+        <v>926</v>
       </c>
       <c r="D8" s="1">
-        <v>1205</v>
+        <v>1035</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="1"/>
-        <v>9.3333333333333339</v>
+        <v>9.4333333333333336</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>12.083333333333334</v>
+        <v>10.583333333333334</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>1020</v>
+        <v>720</v>
       </c>
       <c r="D9" s="1">
-        <v>1252</v>
+        <v>952</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
-        <v>10.333333333333334</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>12.866666666666667</v>
+        <v>9.8666666666666671</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>1006</v>
+        <v>820</v>
       </c>
       <c r="D10" s="1">
-        <v>1235</v>
+        <v>1052</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="1"/>
-        <v>10.1</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>12.583333333333334</v>
+        <v>10.866666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>1100</v>
+        <v>920</v>
       </c>
       <c r="D11" s="1">
-        <v>1311</v>
+        <v>1205</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>13.183333333333334</v>
+        <v>12.083333333333334</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>1141</v>
+        <v>1020</v>
       </c>
       <c r="D12" s="1">
-        <v>1411</v>
+        <v>1252</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
-        <v>11.683333333333334</v>
+        <v>10.333333333333334</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>14.183333333333334</v>
+        <v>12.866666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>1300</v>
+        <v>1220</v>
       </c>
       <c r="D13" s="1">
-        <v>1511</v>
+        <v>1452</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12.333333333333334</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>15.183333333333334</v>
+        <v>14.866666666666667</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1">
-        <v>1341</v>
+        <v>1006</v>
       </c>
       <c r="D14" s="1">
-        <v>1611</v>
+        <v>1235</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="1"/>
-        <v>13.683333333333334</v>
+        <v>10.1</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>16.183333333333334</v>
+        <v>12.583333333333334</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>1302</v>
+        <v>1100</v>
       </c>
       <c r="D15" s="1">
-        <v>1404</v>
+        <v>1311</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>13.033333333333333</v>
+        <v>11</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
-        <v>14.066666666666666</v>
+        <v>13.183333333333334</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>1402</v>
+        <v>4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1141</v>
       </c>
       <c r="D16" s="1">
-        <v>1604</v>
+        <v>1411</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" ref="E16:E31" si="2">ROUNDDOWN(C16/100,0) +MOD(C16,100)/60</f>
-        <v>14.033333333333333</v>
+        <f t="shared" si="1"/>
+        <v>11.683333333333334</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>16.066666666666666</v>
+        <v>14.183333333333334</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
-        <v>1502</v>
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1300</v>
       </c>
       <c r="D17" s="1">
-        <v>1704</v>
+        <v>1511</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="2"/>
-        <v>15.033333333333333</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>17.066666666666666</v>
+        <v>15.183333333333334</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>1602</v>
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1341</v>
       </c>
       <c r="D18" s="1">
-        <v>1804</v>
+        <v>1611</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="2"/>
-        <v>16.033333333333335</v>
+        <f t="shared" si="1"/>
+        <v>13.683333333333334</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
-        <v>18.066666666666666</v>
+        <v>16.183333333333334</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
-        <v>1408</v>
+        <v>1302</v>
       </c>
       <c r="D19" s="1">
-        <v>1522</v>
+        <v>1404</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="2"/>
-        <v>14.133333333333333</v>
+        <f t="shared" si="1"/>
+        <v>13.033333333333333</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
-        <v>15.366666666666667</v>
+        <v>14.066666666666666</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1416</v>
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>1402</v>
       </c>
       <c r="D20" s="1">
-        <v>1548</v>
+        <v>1604</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="2"/>
-        <v>14.266666666666667</v>
+        <f t="shared" ref="E20:E38" si="2">ROUNDDOWN(C20/100,0) +MOD(C20,100)/60</f>
+        <v>14.033333333333333</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
-        <v>15.8</v>
+        <v>16.066666666666666</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1438</v>
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>1502</v>
       </c>
       <c r="D21" s="1">
-        <v>1553</v>
+        <v>1704</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="2"/>
-        <v>14.633333333333333</v>
+        <v>15.033333333333333</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
-        <v>15.883333333333333</v>
+        <v>17.066666666666666</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1508</v>
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>1602</v>
       </c>
       <c r="D22" s="1">
-        <v>1622</v>
+        <v>1804</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="2"/>
-        <v>15.133333333333333</v>
+        <v>16.033333333333335</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
-        <v>16.366666666666667</v>
+        <v>18.066666666666666</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1">
-        <v>1516</v>
+        <v>1408</v>
       </c>
       <c r="D23" s="1">
-        <v>1648</v>
+        <v>1522</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="2"/>
-        <v>15.266666666666667</v>
+        <v>14.133333333333333</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="0"/>
-        <v>16.8</v>
+        <v>15.366666666666667</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1">
-        <v>1608</v>
+        <v>1416</v>
       </c>
       <c r="D24" s="1">
-        <v>1722</v>
+        <v>1548</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
-        <v>16.133333333333333</v>
+        <v>14.266666666666667</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="0"/>
-        <v>17.366666666666667</v>
+        <v>15.8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25" s="1">
-        <v>1616</v>
+        <v>1438</v>
       </c>
       <c r="D25" s="1">
-        <v>1748</v>
+        <v>1553</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>16.266666666666666</v>
+        <v>14.633333333333333</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="0"/>
-        <v>17.8</v>
+        <v>15.883333333333333</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C26" s="1">
-        <v>1638</v>
+        <v>1508</v>
       </c>
       <c r="D26" s="1">
-        <v>1753</v>
+        <v>1622</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="2"/>
-        <v>16.633333333333333</v>
+        <v>15.133333333333333</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="0"/>
-        <v>17.883333333333333</v>
+        <v>16.366666666666667</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C27" s="1">
-        <v>1708</v>
+        <v>1516</v>
       </c>
       <c r="D27" s="1">
-        <v>1822</v>
+        <v>1648</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="2"/>
-        <v>17.133333333333333</v>
+        <v>15.266666666666667</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="0"/>
-        <v>18.366666666666667</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
-        <v>1716</v>
+        <v>1608</v>
       </c>
       <c r="D28" s="1">
-        <v>1848</v>
+        <v>1722</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="2"/>
-        <v>17.266666666666666</v>
+        <v>16.133333333333333</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="0"/>
-        <v>18.8</v>
+        <v>17.366666666666667</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1">
-        <v>1738</v>
+        <v>1616</v>
       </c>
       <c r="D29" s="1">
-        <v>1853</v>
+        <v>1748</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="2"/>
-        <v>17.633333333333333</v>
+        <v>16.266666666666666</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="0"/>
-        <v>18.883333333333333</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1">
-        <v>1808</v>
+        <v>1638</v>
       </c>
       <c r="D30" s="1">
-        <v>1922</v>
+        <v>1753</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="2"/>
-        <v>18.133333333333333</v>
+        <v>16.633333333333333</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="0"/>
-        <v>19.366666666666667</v>
+        <v>17.883333333333333</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C31" s="1">
+        <v>1708</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1822</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="2"/>
+        <v>17.133333333333333</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="0"/>
+        <v>18.366666666666667</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1716</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1848</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="2"/>
+        <v>17.266666666666666</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="0"/>
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1738</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1853</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="2"/>
+        <v>17.633333333333333</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="0"/>
+        <v>18.883333333333333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1808</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1922</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="2"/>
+        <v>18.133333333333333</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="0"/>
+        <v>19.366666666666667</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1816</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1948</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="2"/>
+        <v>18.266666666666666</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="0"/>
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1838</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1953</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="2"/>
+        <v>18.633333333333333</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="0"/>
+        <v>19.883333333333333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1908</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="2"/>
+        <v>19.133333333333333</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="0"/>
+        <v>20.366666666666667</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1">
         <v>1959</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D38" s="1">
         <f>711+2400</f>
         <v>3111</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E38" s="2">
         <f t="shared" si="2"/>
         <v>19.983333333333334</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F38" s="2">
         <f t="shared" si="0"/>
         <v>31.183333333333334</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
         <v>9</v>
       </c>
-      <c r="B32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="C39" s="1">
         <v>1759</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D39" s="1">
         <v>1853</v>
       </c>
-      <c r="E32" s="2">
-        <f t="shared" ref="E32:E40" si="3">ROUNDDOWN(C32/100,0) +MOD(C32,100)/60</f>
+      <c r="E39" s="2">
+        <f t="shared" ref="E39:E50" si="3">ROUNDDOWN(C39/100,0) +MOD(C39,100)/60</f>
         <v>17.983333333333334</v>
       </c>
-      <c r="F32" s="2">
-        <f t="shared" ref="F32:F40" si="4">ROUNDDOWN(D32/100,0) +MOD(D32,100)/60</f>
+      <c r="F39" s="2">
+        <f t="shared" ref="F39:F50" si="4">ROUNDDOWN(D39/100,0) +MOD(D39,100)/60</f>
         <v>18.883333333333333</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
         <v>9</v>
       </c>
-      <c r="B33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="C40" s="1">
         <v>1559</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D40" s="1">
         <v>1653</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E40" s="2">
         <f t="shared" si="3"/>
         <v>15.983333333333333</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F40" s="2">
         <f t="shared" si="4"/>
         <v>16.883333333333333</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
         <v>9</v>
       </c>
-      <c r="B34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="C41" s="1">
         <v>1734</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D41" s="1">
         <v>1828</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E41" s="2">
         <f t="shared" si="3"/>
         <v>17.566666666666666</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F41" s="2">
         <f t="shared" si="4"/>
         <v>18.466666666666665</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="1">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="1">
         <v>1913</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D42" s="1">
         <f>537+2400</f>
         <v>2937</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E42" s="2">
         <f t="shared" si="3"/>
         <v>19.216666666666665</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F42" s="2">
         <f t="shared" si="4"/>
         <v>29.616666666666667</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="1">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1">
         <v>600</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D43" s="1">
         <v>650</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E43" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F43" s="2">
         <f t="shared" si="4"/>
         <v>6.833333333333333</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1">
         <v>700</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D44" s="1">
         <v>750</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E44" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F44" s="2">
         <f t="shared" si="4"/>
         <v>7.833333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" s="1">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1">
         <v>710</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D45" s="1">
         <v>800</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E45" s="2">
         <f t="shared" si="3"/>
         <v>7.166666666666667</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F45" s="2">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="1">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1">
         <v>810</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D46" s="1">
         <v>902</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E46" s="2">
         <f t="shared" si="3"/>
         <v>8.1666666666666661</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F46" s="2">
         <f t="shared" si="4"/>
         <v>9.0333333333333332</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="1">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1">
         <v>1010</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D47" s="1">
         <v>1102</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E47" s="2">
         <f t="shared" si="3"/>
         <v>10.166666666666666</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F47" s="2">
         <f t="shared" si="4"/>
         <v>11.033333333333333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1508</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1728</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="3"/>
+        <v>15.133333333333333</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" si="4"/>
+        <v>17.466666666666665</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1608</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1828</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="3"/>
+        <v>16.133333333333333</v>
+      </c>
+      <c r="F49" s="2">
+        <f t="shared" si="4"/>
+        <v>18.466666666666665</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1808</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2028</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="3"/>
+        <v>18.133333333333333</v>
+      </c>
+      <c r="F50" s="2">
+        <f t="shared" si="4"/>
+        <v>20.466666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -1380,7 +1600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61207BC-DC5C-45B2-AE5F-A7402D7181EA}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1388,15 +1608,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>900</v>
@@ -1404,7 +1624,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>800</v>
@@ -1412,7 +1632,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>700</v>
@@ -1420,7 +1640,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>600</v>
@@ -1428,7 +1648,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -1436,7 +1656,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>400</v>
@@ -1444,7 +1664,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>200</v>
@@ -1452,7 +1672,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>300</v>
@@ -1460,7 +1680,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>100</v>

</xml_diff>

<commit_message>
Working on using clipboard paste, rather than CSV file import. This gets the text/html in Firefox.
</commit_message>
<xml_diff>
--- a/Bernina day timetable.xlsx
+++ b/Bernina day timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ba76bc22b2fda58/Documents/Holiday 2024 Interrail/ZigZagTimetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64E9557A-8B2B-43E2-AE1A-6EF87906A031}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56BFF113-FC62-4017-8BC6-9712E7483316}"/>
   <bookViews>
-    <workbookView xWindow="3386" yWindow="5357" windowWidth="18823" windowHeight="10234" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
+    <workbookView xWindow="81360" yWindow="2295" windowWidth="18240" windowHeight="12030" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Direct trains" sheetId="1" r:id="rId1"/>
@@ -480,13 +480,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C10AF06-4BAA-4E39-BA8A-BDC99B314CB9}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="9.23046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.23046875" style="1"/>
     <col min="5" max="6" width="9.23046875" style="2"/>
   </cols>

</xml_diff>

<commit_message>
Pastes one timetable using clipboard. It works out the station coordinates from the order the timetable entries are listed. Includes the precise time in small vertical writing. This may look better if 'printed' from the browser to a PDF file.
</commit_message>
<xml_diff>
--- a/Bernina day timetable.xlsx
+++ b/Bernina day timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ba76bc22b2fda58/Documents/Holiday 2024 Interrail/ZigZagTimetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56BFF113-FC62-4017-8BC6-9712E7483316}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D479EF-9936-48F8-9994-ADD45AF84014}"/>
   <bookViews>
-    <workbookView xWindow="81360" yWindow="2295" windowWidth="18240" windowHeight="12030" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
+    <workbookView xWindow="77895" yWindow="930" windowWidth="18240" windowHeight="12030" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Direct trains" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="17">
   <si>
     <t>From</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Chur</t>
   </si>
   <si>
-    <t>To direct</t>
-  </si>
-  <si>
     <t>Zurich</t>
   </si>
   <si>
@@ -72,31 +69,33 @@
     <t>Turin</t>
   </si>
   <si>
-    <t>DepHrs</t>
-  </si>
-  <si>
-    <t>ArrHrs</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Depart decimal minnutes</t>
-  </si>
-  <si>
-    <t>Arrive decimal</t>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Depart</t>
+  </si>
+  <si>
+    <t>Arrive</t>
+  </si>
+  <si>
+    <t>StyleClass</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -135,10 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -478,40 +476,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C10AF06-4BAA-4E39-BA8A-BDC99B314CB9}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="A1:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="12.4609375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.23046875" style="1"/>
-    <col min="5" max="6" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -524,16 +518,8 @@
       <c r="D2" s="1">
         <v>705</v>
       </c>
-      <c r="E2" s="2">
-        <f>ROUNDDOWN(C2/100,0) +MOD(C2,100)/60</f>
-        <v>4.9333333333333336</v>
-      </c>
-      <c r="F2" s="2">
-        <f t="shared" ref="F2:F38" si="0">ROUNDDOWN(D2/100,0) +MOD(D2,100)/60</f>
-        <v>7.083333333333333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -546,16 +532,8 @@
       <c r="D3" s="1">
         <v>712</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E19" si="1">ROUNDDOWN(C3/100,0) +MOD(C3,100)/60</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="F3" s="2">
-        <f t="shared" si="0"/>
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -568,16 +546,8 @@
       <c r="D4" s="1">
         <v>850</v>
       </c>
-      <c r="E4" s="2">
-        <f t="shared" si="1"/>
-        <v>7.5166666666666666</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="0"/>
-        <v>8.8333333333333339</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -590,16 +560,8 @@
       <c r="D5" s="1">
         <v>850</v>
       </c>
-      <c r="E5" s="2">
-        <f t="shared" si="1"/>
-        <v>7.5166666666666666</v>
-      </c>
-      <c r="F5" s="2">
-        <f t="shared" si="0"/>
-        <v>8.8333333333333339</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -612,16 +574,8 @@
       <c r="D6" s="1">
         <v>950</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" si="1"/>
-        <v>8.6</v>
-      </c>
-      <c r="F6" s="2">
-        <f t="shared" si="0"/>
-        <v>9.8333333333333339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -634,16 +588,8 @@
       <c r="D7" s="1">
         <v>1000</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" si="1"/>
-        <v>8.9333333333333336</v>
-      </c>
-      <c r="F7" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -656,16 +602,8 @@
       <c r="D8" s="1">
         <v>1035</v>
       </c>
-      <c r="E8" s="2">
-        <f t="shared" si="1"/>
-        <v>9.4333333333333336</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>10.583333333333334</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -678,16 +616,8 @@
       <c r="D9" s="1">
         <v>952</v>
       </c>
-      <c r="E9" s="2">
-        <f t="shared" si="1"/>
-        <v>7.333333333333333</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>9.8666666666666671</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -700,16 +630,8 @@
       <c r="D10" s="1">
         <v>1052</v>
       </c>
-      <c r="E10" s="2">
-        <f t="shared" si="1"/>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>10.866666666666667</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -722,16 +644,8 @@
       <c r="D11" s="1">
         <v>1205</v>
       </c>
-      <c r="E11" s="2">
-        <f t="shared" si="1"/>
-        <v>9.3333333333333339</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>12.083333333333334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -744,16 +658,8 @@
       <c r="D12" s="1">
         <v>1252</v>
       </c>
-      <c r="E12" s="2">
-        <f t="shared" si="1"/>
-        <v>10.333333333333334</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>12.866666666666667</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -766,16 +672,8 @@
       <c r="D13" s="1">
         <v>1452</v>
       </c>
-      <c r="E13" s="2">
-        <f t="shared" si="1"/>
-        <v>12.333333333333334</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="0"/>
-        <v>14.866666666666667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -788,16 +686,8 @@
       <c r="D14" s="1">
         <v>1235</v>
       </c>
-      <c r="E14" s="2">
-        <f t="shared" si="1"/>
-        <v>10.1</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>12.583333333333334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -810,16 +700,8 @@
       <c r="D15" s="1">
         <v>1311</v>
       </c>
-      <c r="E15" s="2">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
-        <v>13.183333333333334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -832,16 +714,8 @@
       <c r="D16" s="1">
         <v>1411</v>
       </c>
-      <c r="E16" s="2">
-        <f t="shared" si="1"/>
-        <v>11.683333333333334</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>14.183333333333334</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -854,16 +728,8 @@
       <c r="D17" s="1">
         <v>1511</v>
       </c>
-      <c r="E17" s="2">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="F17" s="2">
-        <f t="shared" si="0"/>
-        <v>15.183333333333334</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -876,16 +742,8 @@
       <c r="D18" s="1">
         <v>1611</v>
       </c>
-      <c r="E18" s="2">
-        <f t="shared" si="1"/>
-        <v>13.683333333333334</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>16.183333333333334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -898,16 +756,8 @@
       <c r="D19" s="1">
         <v>1404</v>
       </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>13.033333333333333</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>14.066666666666666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -920,16 +770,8 @@
       <c r="D20" s="1">
         <v>1604</v>
       </c>
-      <c r="E20" s="2">
-        <f t="shared" ref="E20:E38" si="2">ROUNDDOWN(C20/100,0) +MOD(C20,100)/60</f>
-        <v>14.033333333333333</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="0"/>
-        <v>16.066666666666666</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -942,16 +784,8 @@
       <c r="D21" s="1">
         <v>1704</v>
       </c>
-      <c r="E21" s="2">
-        <f t="shared" si="2"/>
-        <v>15.033333333333333</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="0"/>
-        <v>17.066666666666666</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -964,21 +798,13 @@
       <c r="D22" s="1">
         <v>1804</v>
       </c>
-      <c r="E22" s="2">
-        <f t="shared" si="2"/>
-        <v>16.033333333333335</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" si="0"/>
-        <v>18.066666666666666</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
         <v>1408</v>
@@ -986,21 +812,13 @@
       <c r="D23" s="1">
         <v>1522</v>
       </c>
-      <c r="E23" s="2">
-        <f t="shared" si="2"/>
-        <v>14.133333333333333</v>
-      </c>
-      <c r="F23" s="2">
-        <f t="shared" si="0"/>
-        <v>15.366666666666667</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <v>1416</v>
@@ -1008,21 +826,13 @@
       <c r="D24" s="1">
         <v>1548</v>
       </c>
-      <c r="E24" s="2">
-        <f t="shared" si="2"/>
-        <v>14.266666666666667</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="0"/>
-        <v>15.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1">
         <v>1438</v>
@@ -1030,21 +840,13 @@
       <c r="D25" s="1">
         <v>1553</v>
       </c>
-      <c r="E25" s="2">
-        <f t="shared" si="2"/>
-        <v>14.633333333333333</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="0"/>
-        <v>15.883333333333333</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1">
         <v>1508</v>
@@ -1052,21 +854,13 @@
       <c r="D26" s="1">
         <v>1622</v>
       </c>
-      <c r="E26" s="2">
-        <f t="shared" si="2"/>
-        <v>15.133333333333333</v>
-      </c>
-      <c r="F26" s="2">
-        <f t="shared" si="0"/>
-        <v>16.366666666666667</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
         <v>1516</v>
@@ -1074,21 +868,13 @@
       <c r="D27" s="1">
         <v>1648</v>
       </c>
-      <c r="E27" s="2">
-        <f t="shared" si="2"/>
-        <v>15.266666666666667</v>
-      </c>
-      <c r="F27" s="2">
-        <f t="shared" si="0"/>
-        <v>16.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
         <v>1608</v>
@@ -1096,21 +882,13 @@
       <c r="D28" s="1">
         <v>1722</v>
       </c>
-      <c r="E28" s="2">
-        <f t="shared" si="2"/>
-        <v>16.133333333333333</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="0"/>
-        <v>17.366666666666667</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
         <v>1616</v>
@@ -1118,21 +896,13 @@
       <c r="D29" s="1">
         <v>1748</v>
       </c>
-      <c r="E29" s="2">
-        <f t="shared" si="2"/>
-        <v>16.266666666666666</v>
-      </c>
-      <c r="F29" s="2">
-        <f t="shared" si="0"/>
-        <v>17.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1">
         <v>1638</v>
@@ -1140,21 +910,13 @@
       <c r="D30" s="1">
         <v>1753</v>
       </c>
-      <c r="E30" s="2">
-        <f t="shared" si="2"/>
-        <v>16.633333333333333</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="0"/>
-        <v>17.883333333333333</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1">
         <v>1708</v>
@@ -1162,21 +924,13 @@
       <c r="D31" s="1">
         <v>1822</v>
       </c>
-      <c r="E31" s="2">
-        <f t="shared" si="2"/>
-        <v>17.133333333333333</v>
-      </c>
-      <c r="F31" s="2">
-        <f t="shared" si="0"/>
-        <v>18.366666666666667</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1">
         <v>1716</v>
@@ -1184,21 +938,13 @@
       <c r="D32" s="1">
         <v>1848</v>
       </c>
-      <c r="E32" s="2">
-        <f t="shared" si="2"/>
-        <v>17.266666666666666</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" si="0"/>
-        <v>18.8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1">
         <v>1738</v>
@@ -1206,21 +952,13 @@
       <c r="D33" s="1">
         <v>1853</v>
       </c>
-      <c r="E33" s="2">
-        <f t="shared" si="2"/>
-        <v>17.633333333333333</v>
-      </c>
-      <c r="F33" s="2">
-        <f t="shared" si="0"/>
-        <v>18.883333333333333</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1">
         <v>1808</v>
@@ -1228,21 +966,13 @@
       <c r="D34" s="1">
         <v>1922</v>
       </c>
-      <c r="E34" s="2">
-        <f t="shared" si="2"/>
-        <v>18.133333333333333</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" si="0"/>
-        <v>19.366666666666667</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="1">
         <v>1816</v>
@@ -1250,21 +980,13 @@
       <c r="D35" s="1">
         <v>1948</v>
       </c>
-      <c r="E35" s="2">
-        <f t="shared" si="2"/>
-        <v>18.266666666666666</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" si="0"/>
-        <v>19.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" s="1">
         <v>1838</v>
@@ -1272,21 +994,13 @@
       <c r="D36" s="1">
         <v>1953</v>
       </c>
-      <c r="E36" s="2">
-        <f t="shared" si="2"/>
-        <v>18.633333333333333</v>
-      </c>
-      <c r="F36" s="2">
-        <f t="shared" si="0"/>
-        <v>19.883333333333333</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" s="1">
         <v>1908</v>
@@ -1294,301 +1008,133 @@
       <c r="D37" s="1">
         <v>2022</v>
       </c>
-      <c r="E37" s="2">
-        <f t="shared" si="2"/>
-        <v>19.133333333333333</v>
-      </c>
-      <c r="F37" s="2">
-        <f t="shared" si="0"/>
-        <v>20.366666666666667</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="1">
+        <v>1508</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1608</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1808</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2059</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1759</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1559</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1734</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1913</v>
+      </c>
+      <c r="D45" s="1">
+        <f>537+2400</f>
+        <v>2937</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="1">
         <v>1959</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D46" s="1">
         <f>711+2400</f>
         <v>3111</v>
-      </c>
-      <c r="E38" s="2">
-        <f t="shared" si="2"/>
-        <v>19.983333333333334</v>
-      </c>
-      <c r="F38" s="2">
-        <f t="shared" si="0"/>
-        <v>31.183333333333334</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1759</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1853</v>
-      </c>
-      <c r="E39" s="2">
-        <f t="shared" ref="E39:E50" si="3">ROUNDDOWN(C39/100,0) +MOD(C39,100)/60</f>
-        <v>17.983333333333334</v>
-      </c>
-      <c r="F39" s="2">
-        <f t="shared" ref="F39:F50" si="4">ROUNDDOWN(D39/100,0) +MOD(D39,100)/60</f>
-        <v>18.883333333333333</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1559</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1653</v>
-      </c>
-      <c r="E40" s="2">
-        <f t="shared" si="3"/>
-        <v>15.983333333333333</v>
-      </c>
-      <c r="F40" s="2">
-        <f t="shared" si="4"/>
-        <v>16.883333333333333</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1734</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1828</v>
-      </c>
-      <c r="E41" s="2">
-        <f t="shared" si="3"/>
-        <v>17.566666666666666</v>
-      </c>
-      <c r="F41" s="2">
-        <f t="shared" si="4"/>
-        <v>18.466666666666665</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1913</v>
-      </c>
-      <c r="D42" s="1">
-        <f>537+2400</f>
-        <v>2937</v>
-      </c>
-      <c r="E42" s="2">
-        <f t="shared" si="3"/>
-        <v>19.216666666666665</v>
-      </c>
-      <c r="F42" s="2">
-        <f t="shared" si="4"/>
-        <v>29.616666666666667</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" s="1">
-        <v>600</v>
-      </c>
-      <c r="D43" s="1">
-        <v>650</v>
-      </c>
-      <c r="E43" s="2">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="F43" s="2">
-        <f t="shared" si="4"/>
-        <v>6.833333333333333</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="1">
-        <v>700</v>
-      </c>
-      <c r="D44" s="1">
-        <v>750</v>
-      </c>
-      <c r="E44" s="2">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="F44" s="2">
-        <f t="shared" si="4"/>
-        <v>7.833333333333333</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="1">
-        <v>710</v>
-      </c>
-      <c r="D45" s="1">
-        <v>800</v>
-      </c>
-      <c r="E45" s="2">
-        <f t="shared" si="3"/>
-        <v>7.166666666666667</v>
-      </c>
-      <c r="F45" s="2">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C46" s="1">
-        <v>810</v>
-      </c>
-      <c r="D46" s="1">
-        <v>902</v>
-      </c>
-      <c r="E46" s="2">
-        <f t="shared" si="3"/>
-        <v>8.1666666666666661</v>
-      </c>
-      <c r="F46" s="2">
-        <f t="shared" si="4"/>
-        <v>9.0333333333333332</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" t="s">
-        <v>2</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1010</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1102</v>
-      </c>
-      <c r="E47" s="2">
-        <f t="shared" si="3"/>
-        <v>10.166666666666666</v>
-      </c>
-      <c r="F47" s="2">
-        <f t="shared" si="4"/>
-        <v>11.033333333333333</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1508</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1728</v>
-      </c>
-      <c r="E48" s="2">
-        <f t="shared" si="3"/>
-        <v>15.133333333333333</v>
-      </c>
-      <c r="F48" s="2">
-        <f t="shared" si="4"/>
-        <v>17.466666666666665</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1608</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1828</v>
-      </c>
-      <c r="E49" s="2">
-        <f t="shared" si="3"/>
-        <v>16.133333333333333</v>
-      </c>
-      <c r="F49" s="2">
-        <f t="shared" si="4"/>
-        <v>18.466666666666665</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1808</v>
-      </c>
-      <c r="D50" s="1">
-        <v>2028</v>
-      </c>
-      <c r="E50" s="2">
-        <f t="shared" si="3"/>
-        <v>18.133333333333333</v>
-      </c>
-      <c r="F50" s="2">
-        <f t="shared" si="4"/>
-        <v>20.466666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -1606,17 +1152,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>14</v>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>900</v>
@@ -1624,7 +1170,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>800</v>
@@ -1632,7 +1178,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>700</v>
@@ -1664,7 +1210,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>200</v>

</xml_diff>

<commit_message>
Added actual timetables to different places. Tidied up CSS
</commit_message>
<xml_diff>
--- a/Bernina day timetable.xlsx
+++ b/Bernina day timetable.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ba76bc22b2fda58/Documents/Holiday 2024 Interrail/ZigZagTimetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D479EF-9936-48F8-9994-ADD45AF84014}"/>
+  <xr:revisionPtr revIDLastSave="576" documentId="8_{B7A3A716-4575-4322-8F69-936EA9E82F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1B541CC-8DBF-4A56-A3D7-ECA8C3ED7A18}"/>
   <bookViews>
-    <workbookView xWindow="77895" yWindow="930" windowWidth="18240" windowHeight="12030" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
+    <workbookView xWindow="65010" yWindow="15480" windowWidth="15840" windowHeight="15045" activeTab="1" xr2:uid="{8569A97E-35FE-416B-B166-13311120B0FD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Direct trains" sheetId="1" r:id="rId1"/>
-    <sheet name="Stations" sheetId="2" r:id="rId2"/>
+    <sheet name="Bernina" sheetId="1" r:id="rId1"/>
+    <sheet name="Budapest" sheetId="2" r:id="rId2"/>
+    <sheet name="Nice" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="37">
   <si>
     <t>From</t>
   </si>
@@ -66,15 +67,6 @@
     <t>Basel</t>
   </si>
   <si>
-    <t>Turin</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>To</t>
   </si>
   <si>
@@ -88,14 +80,84 @@
   </si>
   <si>
     <t>Hamburg</t>
+  </si>
+  <si>
+    <t>minor</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Giffnock</t>
+  </si>
+  <si>
+    <t>Bruxelles</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>Dresden</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>Vienna</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Augsburg</t>
+  </si>
+  <si>
+    <t>Koeln</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>change station</t>
+  </si>
+  <si>
+    <t>flughavfen ?</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>important</t>
+  </si>
+  <si>
+    <t>Nice</t>
+  </si>
+  <si>
+    <t>Williamwood</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>routeA</t>
+  </si>
+  <si>
+    <t>routeB</t>
+  </si>
+  <si>
+    <t>routeC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#0000"/>
+    <numFmt numFmtId="165" formatCode="0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -134,10 +196,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C10AF06-4BAA-4E39-BA8A-BDC99B314CB9}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="A1:D46"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -493,16 +557,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
@@ -555,10 +619,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>731</v>
+        <v>813</v>
       </c>
       <c r="D5" s="1">
-        <v>850</v>
+        <v>935</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -939,7 +1003,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -953,7 +1017,7 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -967,7 +1031,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -981,7 +1045,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -995,7 +1059,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1009,7 +1073,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1022,8 +1086,11 @@
       <c r="D38" s="1">
         <v>1728</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>5</v>
       </c>
@@ -1036,8 +1103,11 @@
       <c r="D39" s="1">
         <v>1828</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1050,13 +1120,16 @@
       <c r="D40" s="1">
         <v>2028</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C41" s="1">
         <v>2059</v>
@@ -1064,8 +1137,11 @@
       <c r="D41" s="1">
         <v>3136</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1078,8 +1154,11 @@
       <c r="D42" s="1">
         <v>1853</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1092,8 +1171,11 @@
       <c r="D43" s="1">
         <v>1653</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1106,8 +1188,11 @@
       <c r="D44" s="1">
         <v>1828</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1121,8 +1206,11 @@
         <f>537+2400</f>
         <v>2937</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>6</v>
       </c>
@@ -1144,92 +1232,1405 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61207BC-DC5C-45B2-AE5F-A7402D7181EA}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="9.23046875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.23046875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>711</v>
+      </c>
+      <c r="D3" s="1">
+        <v>728</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>744</v>
+      </c>
+      <c r="D4" s="1">
+        <v>759</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>814</v>
+      </c>
+      <c r="D5" s="1">
+        <v>830</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>426</v>
+      </c>
+      <c r="D6" s="1">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>607</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1">
+        <v>809</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1321</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1">
+        <v>816</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1113</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1">
+        <v>901</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1205</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1104</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1131</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1031</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1">
+        <v>825</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1117</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1025</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1317</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1625</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1931</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1225</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1531</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1425</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1325</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1515</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1425</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1615</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1623</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1815</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1725</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1915</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1420</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1740</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1749</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2041</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1549</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1841</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1949</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2240</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1555</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1953</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1710</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2053</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1755</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2153</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1911</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2253</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1555</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2104</v>
+      </c>
+      <c r="F32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1622</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2131</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1903</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3413</v>
+      </c>
+      <c r="E34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2302</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3302</v>
+      </c>
+      <c r="E35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1034</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1258</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2153</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1401</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2047</v>
+      </c>
+      <c r="E38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2140</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2402</v>
+      </c>
+      <c r="E39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1201</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1847</v>
+      </c>
+      <c r="E40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1621</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2305</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1942</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2202</v>
+      </c>
+      <c r="E42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2037</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2302</v>
+      </c>
+      <c r="E43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2140</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2402</v>
+      </c>
+      <c r="E44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0571A916-ECF0-4906-B08D-A56D1BFBFE44}">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="9.23046875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.23046875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3">
+        <v>638</v>
+      </c>
+      <c r="D2" s="3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>708</v>
+      </c>
+      <c r="D3" s="3">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3">
+        <v>600</v>
+      </c>
+      <c r="D4" s="3">
+        <v>649</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3">
+        <v>645</v>
+      </c>
+      <c r="D5" s="3">
+        <v>737</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3">
+        <v>715</v>
+      </c>
+      <c r="D6" s="3">
+        <v>807</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2330</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2417</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3">
+        <v>600</v>
+      </c>
+      <c r="D8" s="3">
+        <v>648</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>645</v>
+      </c>
+      <c r="D9" s="3">
+        <v>737</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>715</v>
+      </c>
+      <c r="D10" s="3">
+        <v>807</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2330</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2419</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="3">
+        <v>600</v>
+      </c>
+      <c r="D12" s="3">
+        <v>629</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3">
+        <v>224</v>
+      </c>
+      <c r="D13" s="3">
+        <v>311</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3">
+        <v>354</v>
+      </c>
+      <c r="D14" s="3">
+        <v>447</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3">
+        <v>435</v>
+      </c>
+      <c r="D15" s="3">
+        <v>533</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3">
+        <v>535</v>
+      </c>
+      <c r="D16" s="3">
+        <v>610</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3">
+        <v>634</v>
+      </c>
+      <c r="D17" s="3">
+        <v>657</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3">
+        <v>702</v>
+      </c>
+      <c r="D18" s="3">
+        <v>726</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3">
+        <v>731</v>
+      </c>
+      <c r="D19" s="3">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="3">
+        <v>810</v>
+      </c>
+      <c r="D20" s="3">
+        <v>835</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3">
+        <v>841</v>
+      </c>
+      <c r="D21" s="3">
+        <v>905</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="3">
+        <v>928</v>
+      </c>
+      <c r="D22" s="3">
+        <v>952</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="3">
+        <v>428</v>
+      </c>
+      <c r="D23" s="3">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="3">
+        <v>533</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="3">
+        <v>629</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="3">
+        <v>736</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="3">
+        <v>838</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3">
+        <v>540</v>
+      </c>
+      <c r="D28" s="3">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="3">
+        <v>548</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="3">
+        <v>623</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="3">
+        <v>626</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="3">
         <v>700</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>100</v>
+      <c r="D32" s="3">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1024</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1358</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1131</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1231</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1331</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1648</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1431</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1531</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1410</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1722</v>
+      </c>
+      <c r="D40" s="3">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2051</v>
+      </c>
+      <c r="D41" s="3">
+        <v>3325</v>
+      </c>
+      <c r="E41" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>